<commit_message>
updates to psychometrics paper following feedback
</commit_message>
<xml_diff>
--- a/04_papers/SEM_layout.xlsx
+++ b/04_papers/SEM_layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/foreilly/Documents/GitHub/levante-pilots/04_paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/foreilly/Documents/GitHub/levante-pilots/04_papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ADEE2E-FDFE-CD4E-A999-800D95A40D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277E5ECF-3ED9-7C48-9E16-8393F9791257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16620" xr2:uid="{93E1DCAB-3691-2E4C-AB4F-4E1A49D437BD}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>language</t>
   </si>
   <si>
-    <t>log_age_c</t>
-  </si>
-  <si>
     <t>matrix</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>vocab</t>
+  </si>
+  <si>
+    <t>age_c</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +463,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -485,25 +485,25 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>11</v>
-      </c>
-      <c r="M7" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>